<commit_message>
Added units to the graphs
</commit_message>
<xml_diff>
--- a/test/test_results.xlsx
+++ b/test/test_results.xlsx
@@ -170,11 +170,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -217,7 +216,7 @@
             </a:pPr>
             <a:r>
               <a:rPr/>
-              <a:t>Memory Usage</a:t>
+              <a:t>Memory Usage [MB]</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -1040,11 +1039,11 @@
         </c:ser>
         <c:marker val="0"/>
         <c:smooth val="0"/>
-        <c:axId val="511722081"/>
-        <c:axId val="511722082"/>
+        <c:axId val="511722113"/>
+        <c:axId val="511722114"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="511722081"/>
+        <c:axId val="511722113"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1087,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="511722082"/>
+        <c:crossAx val="511722114"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1097,7 +1096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="511722082"/>
+        <c:axId val="511722114"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1152,7 +1151,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="511722081"/>
+        <c:crossAx val="511722113"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1278,7 +1277,7 @@
             </a:r>
             <a:r>
               <a:rPr/>
-              <a:t>me</a:t>
+              <a:t>me [ms]</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -2087,6 +2086,14 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:marker val="0"/>
         <c:smooth val="0"/>
         <c:axId val="511722103"/>
@@ -2324,7 +2331,7 @@
             </a:pPr>
             <a:r>
               <a:rPr/>
-              <a:t>Simple Ops</a:t>
+              <a:t>Simple Ops [ms]</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -3133,6 +3140,14 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:marker val="0"/>
         <c:smooth val="0"/>
         <c:axId val="511722101"/>
@@ -3374,7 +3389,7 @@
             </a:r>
             <a:r>
               <a:rPr/>
-              <a:t>Ops</a:t>
+              <a:t>Ops [ms]</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -4183,6 +4198,14 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:marker val="0"/>
         <c:smooth val="0"/>
         <c:axId val="511722105"/>
@@ -6753,7 +6776,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>158748</xdr:colOff>
+      <xdr:colOff>158747</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>88898</xdr:rowOff>
     </xdr:from>
@@ -6791,7 +6814,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>101595</xdr:colOff>
+      <xdr:colOff>101594</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>124485</xdr:rowOff>
     </xdr:to>
@@ -6817,7 +6840,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>101595</xdr:colOff>
+      <xdr:colOff>101594</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>88898</xdr:rowOff>
     </xdr:from>
@@ -7482,7 +7505,7 @@
       <c r="I2" s="3">
         <v>0.02</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>0.02</v>
       </c>
       <c r="K2" s="3">
@@ -7494,7 +7517,7 @@
       <c r="M2" s="3">
         <v>0.01</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>0.12</v>
       </c>
       <c r="O2" s="3">
@@ -7535,7 +7558,7 @@
       <c r="I3" s="3">
         <v>0.14999999999999999</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>0.080000000000000002</v>
       </c>
       <c r="K3" s="3">
@@ -7547,7 +7570,7 @@
       <c r="M3" s="3">
         <v>0.029999999999999999</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>0.59999999999999998</v>
       </c>
       <c r="O3" s="3">
@@ -7588,7 +7611,7 @@
       <c r="I4" s="3">
         <v>0.14999999999999999</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>0.17999999999999999</v>
       </c>
       <c r="K4" s="3">
@@ -7600,7 +7623,7 @@
       <c r="M4" s="3">
         <v>0.070000000000000007</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>1.2</v>
       </c>
       <c r="O4" s="3">
@@ -7641,7 +7664,7 @@
       <c r="I5" s="3">
         <v>1.1899999999999999</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>1</v>
       </c>
       <c r="K5" s="3">
@@ -7653,7 +7676,7 @@
       <c r="M5" s="3">
         <v>0.38</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>5.9299999999999997</v>
       </c>
       <c r="O5" s="3">
@@ -7694,7 +7717,7 @@
       <c r="I6" s="3">
         <v>2.04</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>2.0499999999999998</v>
       </c>
       <c r="K6" s="3">
@@ -7706,7 +7729,7 @@
       <c r="M6" s="3">
         <v>0.70999999999999996</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>11.93</v>
       </c>
       <c r="O6" s="3">
@@ -7871,7 +7894,7 @@
       <c r="O9" s="3">
         <v>364.56</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>1267.3</v>
       </c>
       <c r="Q9" s="3">
@@ -7912,7 +7935,7 @@
       <c r="K10" s="3">
         <v>95.280000000000001</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>257.94</v>
       </c>
       <c r="M10" s="3">
@@ -8077,7 +8100,7 @@
       <c r="M13" s="3">
         <v>352.43000000000001</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <v>4709.6700000000001</v>
       </c>
       <c r="O13" s="3">

</xml_diff>